<commit_message>
LV_Activities Changes - 26 June 2024
</commit_message>
<xml_diff>
--- a/TestData/TMT0047476_VerifyActivityAccessRelatedFunctionalityOnCompanyDetailPage.xlsx
+++ b/TestData/TMT0047476_VerifyActivityAccessRelatedFunctionalityOnCompanyDetailPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E18B35B-F872-4BF9-BF72-BE248614FC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441A5CB0-F19B-469E-BB99-61E261496293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>James Craven</t>
-  </si>
-  <si>
     <t>CompanyName</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Module Name</t>
   </si>
   <si>
-    <t>FR Capital Provider</t>
-  </si>
-  <si>
     <t>Tab</t>
   </si>
   <si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>Print</t>
+  </si>
+  <si>
+    <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>ActivityCompany</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,26 +568,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -611,17 +611,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -653,12 +653,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -678,12 +678,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,18 +706,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -748,54 +748,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -823,30 +823,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -870,30 +870,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -917,32 +917,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -954,7 +954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95D2294-D185-4874-A4CE-34B75A6DBCF8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -965,12 +965,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LV Activitiy changes - 19 July 2024
</commit_message>
<xml_diff>
--- a/TestData/TMT0047476_VerifyActivityAccessRelatedFunctionalityOnCompanyDetailPage.xlsx
+++ b/TestData/TMT0047476_VerifyActivityAccessRelatedFunctionalityOnCompanyDetailPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441A5CB0-F19B-469E-BB99-61E261496293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73CA895-94DD-460B-8929-AF2EEC722921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Companies</t>
   </si>
   <si>
-    <t>The Activity has been saved successfully.</t>
-  </si>
-  <si>
     <t>SuccessPopUpMsg</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>ActivityCompany</t>
+  </si>
+  <si>
+    <t>Record saved!</t>
   </si>
 </sst>
 </file>
@@ -568,26 +568,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -611,17 +611,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -714,7 +714,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -769,7 +769,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -777,7 +777,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -786,16 +786,16 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47E1313-6700-419E-B447-93C25ACEE135}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,30 +823,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -873,27 +873,27 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -917,32 +917,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +970,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>